<commit_message>
Company cases - latest changes - 28th Mar 2023
</commit_message>
<xml_diff>
--- a/TestData/TMTT0014212_VerifyTheUserIsAbleToAddNewSectorOnContactCompanyOpportunityEngagementPages.xlsx
+++ b/TestData/TMTT0014212_VerifyTheUserIsAbleToAddNewSectorOnContactCompanyOpportunityEngagementPages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20392"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBBB789-E611-42F3-A449-798A3E611164}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9377461B-4C7C-4BE9-8214-98B4C8C1BEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="128">
   <si>
     <t>CompanyType</t>
   </si>
@@ -106,9 +106,6 @@
     <t>Capital Provider</t>
   </si>
   <si>
-    <t>TestCapitalProvider</t>
-  </si>
-  <si>
     <t>Asset Manager</t>
   </si>
   <si>
@@ -133,21 +130,9 @@
     <t>Tertiary Sector</t>
   </si>
   <si>
-    <t>Eve Apollonio</t>
-  </si>
-  <si>
-    <t>Andrea Ghittino</t>
-  </si>
-  <si>
-    <t>Alex Hughes</t>
-  </si>
-  <si>
     <t>Users</t>
   </si>
   <si>
-    <t>Vijay Kumar</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -175,12 +160,6 @@
     <t>ExternalContact</t>
   </si>
   <si>
-    <t>Test ExternalContact</t>
-  </si>
-  <si>
-    <t>testJames@email.com</t>
-  </si>
-  <si>
     <t>(541) 754-3010</t>
   </si>
   <si>
@@ -425,13 +404,25 @@
   </si>
   <si>
     <t>Danielle Morello</t>
+  </si>
+  <si>
+    <t>TestNewCapitalProvider</t>
+  </si>
+  <si>
+    <t>TestNew</t>
+  </si>
+  <si>
+    <t>TestNew ExternalContact</t>
+  </si>
+  <si>
+    <t>testnewexternalcontact@email.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,6 +440,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -471,21 +470,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -767,7 +768,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -824,8 +825,8 @@
       <c r="M1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>26</v>
+      <c r="N1" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -833,7 +834,7 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>124</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -854,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J2" t="s">
         <v>16</v>
@@ -868,8 +869,8 @@
       <c r="M2" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>27</v>
+      <c r="N2" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -881,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21B8287F-D5E9-440C-9969-6C273E798C8D}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -901,45 +902,45 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>49</v>
+        <v>126</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -973,10 +974,10 @@
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="14.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="14.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="21" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="27" bestFit="1" customWidth="1"/>
@@ -987,376 +988,376 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="O1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="P1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="T1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="V1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="W1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="X1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="AA1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L2" t="s">
         <v>83</v>
       </c>
-      <c r="B2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="M2" t="s">
         <v>84</v>
       </c>
-      <c r="D2" t="s">
+      <c r="N2" t="s">
         <v>85</v>
       </c>
-      <c r="E2" t="s">
+      <c r="O2" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F2" t="s">
+      <c r="P2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="R2" t="s">
         <v>87</v>
       </c>
-      <c r="G2" t="s">
+      <c r="S2" t="s">
         <v>87</v>
       </c>
-      <c r="H2" t="s">
+      <c r="T2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="I2" t="s">
-        <v>87</v>
-      </c>
-      <c r="J2" t="s">
-        <v>87</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="U2" t="s">
+        <v>40</v>
+      </c>
+      <c r="V2" t="s">
         <v>89</v>
       </c>
-      <c r="L2" t="s">
+      <c r="W2" t="s">
         <v>90</v>
       </c>
-      <c r="M2" t="s">
+      <c r="X2" t="s">
         <v>91</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Y2" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="Z2" t="s">
         <v>93</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="AA2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD2" t="s">
         <v>94</v>
       </c>
-      <c r="S2" t="s">
+      <c r="AE2" t="s">
         <v>94</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="U2" t="s">
-        <v>45</v>
-      </c>
-      <c r="V2" t="s">
-        <v>96</v>
-      </c>
-      <c r="W2" t="s">
-        <v>97</v>
-      </c>
-      <c r="X2" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I3" t="s">
+        <v>80</v>
+      </c>
+      <c r="J3" t="s">
+        <v>80</v>
+      </c>
+      <c r="K3" t="s">
+        <v>82</v>
+      </c>
+      <c r="L3" t="s">
         <v>83</v>
       </c>
-      <c r="B3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="M3" t="s">
+        <v>84</v>
+      </c>
+      <c r="N3" t="s">
+        <v>96</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F3" t="s">
+      <c r="P3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="R3" t="s">
         <v>87</v>
       </c>
-      <c r="G3" t="s">
+      <c r="S3" t="s">
         <v>87</v>
       </c>
-      <c r="H3" t="s">
+      <c r="T3" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="I3" t="s">
-        <v>87</v>
-      </c>
-      <c r="J3" t="s">
-        <v>87</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="U3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V3" t="s">
         <v>89</v>
       </c>
-      <c r="L3" t="s">
+      <c r="W3" t="s">
         <v>90</v>
       </c>
-      <c r="M3" t="s">
+      <c r="X3" t="s">
         <v>91</v>
       </c>
-      <c r="N3" t="s">
-        <v>103</v>
-      </c>
-      <c r="O3" s="3" t="s">
+      <c r="Y3" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z3" t="s">
         <v>93</v>
       </c>
-      <c r="P3" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="R3" t="s">
+      <c r="AA3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD3" t="s">
         <v>94</v>
       </c>
-      <c r="S3" t="s">
+      <c r="AE3" t="s">
         <v>94</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="U3" t="s">
-        <v>45</v>
-      </c>
-      <c r="V3" t="s">
-        <v>96</v>
-      </c>
-      <c r="W3" t="s">
-        <v>97</v>
-      </c>
-      <c r="X3" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>104</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>101</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I4" t="s">
+        <v>80</v>
+      </c>
+      <c r="J4" t="s">
+        <v>80</v>
+      </c>
+      <c r="K4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L4" t="s">
         <v>83</v>
       </c>
-      <c r="B4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="M4" t="s">
+        <v>84</v>
+      </c>
+      <c r="N4" t="s">
+        <v>99</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F4" t="s">
+      <c r="P4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="R4" t="s">
         <v>87</v>
       </c>
-      <c r="G4" t="s">
+      <c r="S4" t="s">
         <v>87</v>
       </c>
-      <c r="H4" t="s">
+      <c r="T4" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="I4" t="s">
-        <v>87</v>
-      </c>
-      <c r="J4" t="s">
-        <v>87</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="U4" t="s">
+        <v>40</v>
+      </c>
+      <c r="V4" t="s">
         <v>89</v>
       </c>
-      <c r="L4" t="s">
+      <c r="W4" t="s">
         <v>90</v>
       </c>
-      <c r="M4" t="s">
+      <c r="X4" t="s">
         <v>91</v>
       </c>
-      <c r="N4" t="s">
-        <v>106</v>
-      </c>
-      <c r="O4" s="3" t="s">
+      <c r="Y4" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z4" t="s">
         <v>93</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="R4" t="s">
+      <c r="AA4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD4" t="s">
         <v>94</v>
       </c>
-      <c r="S4" t="s">
+      <c r="AE4" t="s">
         <v>94</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="U4" t="s">
-        <v>45</v>
-      </c>
-      <c r="V4" t="s">
-        <v>96</v>
-      </c>
-      <c r="W4" t="s">
-        <v>97</v>
-      </c>
-      <c r="X4" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>107</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>108</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>101</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1379,12 +1380,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1394,10 +1395,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="A3" sqref="A3:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1407,37 +1408,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1466,54 +1442,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="G2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1525,7 +1501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{260BDF60-7C3B-4898-9BC2-F5F8D9A6360E}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -1537,34 +1513,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1590,30 +1566,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Companies Test data change - 23 Jan 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTT0014212_VerifyTheUserIsAbleToAddNewSectorOnContactCompanyOpportunityEngagementPages.xlsx
+++ b/TestData/TMTT0014212_VerifyTheUserIsAbleToAddNewSectorOnContactCompanyOpportunityEngagementPages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6C3306-51E7-41D7-93BF-9D2B582CFA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300B903A-8055-4C88-A8EA-476D350A9DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="127">
   <si>
     <t>CompanyType</t>
   </si>
@@ -113,9 +113,6 @@
   </si>
   <si>
     <t>123456.0</t>
-  </si>
-  <si>
-    <t>Oscar Aarts</t>
   </si>
   <si>
     <t>Coverage Type</t>
@@ -834,7 +831,7 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -902,45 +899,45 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
         <v>124</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" t="s">
         <v>42</v>
-      </c>
-      <c r="G2" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -988,376 +985,376 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
         <v>76</v>
       </c>
-      <c r="B2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>77</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>78</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>79</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" t="s">
         <v>80</v>
       </c>
-      <c r="G2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K2" t="s">
         <v>81</v>
       </c>
-      <c r="I2" t="s">
-        <v>80</v>
-      </c>
-      <c r="J2" t="s">
-        <v>80</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>82</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>83</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>84</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="R2" t="s">
         <v>86</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="S2" t="s">
         <v>86</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="T2" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="S2" t="s">
-        <v>87</v>
-      </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V2" t="s">
         <v>88</v>
       </c>
-      <c r="U2" t="s">
-        <v>40</v>
-      </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>89</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>90</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>91</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>92</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AD2" t="s">
         <v>93</v>
       </c>
-      <c r="AA2" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>94</v>
-      </c>
       <c r="AE2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J3" t="s">
+        <v>79</v>
+      </c>
+      <c r="K3" t="s">
+        <v>81</v>
+      </c>
+      <c r="L3" t="s">
+        <v>82</v>
+      </c>
+      <c r="M3" t="s">
+        <v>83</v>
+      </c>
+      <c r="N3" t="s">
         <v>95</v>
       </c>
-      <c r="D3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H3" t="s">
-        <v>81</v>
-      </c>
-      <c r="I3" t="s">
-        <v>80</v>
-      </c>
-      <c r="J3" t="s">
-        <v>80</v>
-      </c>
-      <c r="K3" t="s">
-        <v>82</v>
-      </c>
-      <c r="L3" t="s">
-        <v>83</v>
-      </c>
-      <c r="M3" t="s">
-        <v>84</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="O3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="R3" t="s">
+        <v>86</v>
+      </c>
+      <c r="S3" t="s">
+        <v>86</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="U3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V3" t="s">
+        <v>88</v>
+      </c>
+      <c r="W3" t="s">
+        <v>89</v>
+      </c>
+      <c r="X3" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y3" t="s">
         <v>96</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="R3" t="s">
-        <v>87</v>
-      </c>
-      <c r="S3" t="s">
-        <v>87</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="U3" t="s">
-        <v>40</v>
-      </c>
-      <c r="V3" t="s">
-        <v>89</v>
-      </c>
-      <c r="W3" t="s">
-        <v>90</v>
-      </c>
-      <c r="X3" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>97</v>
-      </c>
       <c r="Z3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AD3" t="s">
         <v>93</v>
       </c>
-      <c r="AA3" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>94</v>
-      </c>
       <c r="AE3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I4" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4" t="s">
+        <v>79</v>
+      </c>
+      <c r="K4" t="s">
+        <v>81</v>
+      </c>
+      <c r="L4" t="s">
+        <v>82</v>
+      </c>
+      <c r="M4" t="s">
+        <v>83</v>
+      </c>
+      <c r="N4" t="s">
         <v>98</v>
       </c>
-      <c r="D4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" t="s">
-        <v>80</v>
-      </c>
-      <c r="G4" t="s">
-        <v>80</v>
-      </c>
-      <c r="H4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I4" t="s">
-        <v>80</v>
-      </c>
-      <c r="J4" t="s">
-        <v>80</v>
-      </c>
-      <c r="K4" t="s">
-        <v>82</v>
-      </c>
-      <c r="L4" t="s">
-        <v>83</v>
-      </c>
-      <c r="M4" t="s">
-        <v>84</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="O4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="R4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S4" t="s">
+        <v>86</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="U4" t="s">
+        <v>39</v>
+      </c>
+      <c r="V4" t="s">
+        <v>88</v>
+      </c>
+      <c r="W4" t="s">
+        <v>89</v>
+      </c>
+      <c r="X4" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y4" t="s">
         <v>99</v>
       </c>
-      <c r="O4" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="R4" t="s">
-        <v>87</v>
-      </c>
-      <c r="S4" t="s">
-        <v>87</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="U4" t="s">
-        <v>40</v>
-      </c>
-      <c r="V4" t="s">
-        <v>89</v>
-      </c>
-      <c r="W4" t="s">
-        <v>90</v>
-      </c>
-      <c r="X4" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC4" t="s">
         <v>100</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AD4" t="s">
         <v>93</v>
       </c>
-      <c r="AA4" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>101</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>94</v>
-      </c>
       <c r="AE4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1380,12 +1377,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1397,8 +1394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1408,12 +1405,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1442,54 +1439,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" t="s">
         <v>110</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>111</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
         <v>112</v>
       </c>
-      <c r="E2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" t="s">
         <v>113</v>
-      </c>
-      <c r="G2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1513,34 +1510,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1552,7 +1549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4227CC6F-542E-48BC-82A4-18911F5F4C92}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -1566,30 +1563,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" t="s">
         <v>119</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>120</v>
-      </c>
-      <c r="D2" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>